<commit_message>
Added categories.json and its coupled method initMenuContent
</commit_message>
<xml_diff>
--- a/excel-to-json/data.xlsx
+++ b/excel-to-json/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Carlos\LostInMadrid\lost-in-madrid\excel-to-json\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Carlos\MadridForAll\madrid-for-all\excel-to-json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6BACDB-9414-41A5-BCF4-3C9C985FF32B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CF1E6D-6DEE-4C73-8940-91FBE6F0D5C4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1315,10 +1315,13 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:V23"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">

</xml_diff>

<commit_message>
Added tabs to the table of results
</commit_message>
<xml_diff>
--- a/excel-to-json/data.xlsx
+++ b/excel-to-json/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Carlos\MadridForAll\madrid-for-all\excel-to-json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B48EF1-E9C4-4684-8871-65B8E1224E66}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCC5662-66FF-42E6-B6D4-E5ACCE2597D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="WaysOfContact" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Categories!$A$1:$E$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Categories!$A$1:$E$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Services!$A$1:$F$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="296">
   <si>
     <t>aem@alternativaenmarcha.org</t>
   </si>
@@ -782,18 +782,6 @@
   </si>
   <si>
     <t>Información y orientación laboral</t>
-  </si>
-  <si>
-    <t>Mujer</t>
-  </si>
-  <si>
-    <t>Infancia y jóvenes</t>
-  </si>
-  <si>
-    <t>Familia</t>
-  </si>
-  <si>
-    <t>LGTBIQ+</t>
   </si>
   <si>
     <t>category</t>
@@ -1085,25 +1073,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2400,8 +2383,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4330DA9B-DBFA-4512-8AC8-B56D06C6B546}" name="Table1" displayName="Table1" ref="A1:E11" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:E11" xr:uid="{F2747FD6-900C-4C5E-A9C9-1F8D01AA6874}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4330DA9B-DBFA-4512-8AC8-B56D06C6B546}" name="Table1" displayName="Table1" ref="A1:E7" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:E7" xr:uid="{F2747FD6-900C-4C5E-A9C9-1F8D01AA6874}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8764652D-E4F6-423B-942A-B683684BCE4E}" name="key" dataDxfId="19">
       <calculatedColumnFormula>IF(COUNTA($B2:$E2)&gt;0,CONCATENATE("cat",ROW($A2)-1),"Fill in the labels!")</calculatedColumnFormula>
@@ -2748,7 +2731,7 @@
   </sheetPr>
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="H5" sqref="H5"/>
     </sheetView>
@@ -2760,11 +2743,11 @@
     <col min="11" max="11" width="13.5703125" customWidth="1"/>
     <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.85546875" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="22" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.85546875" customWidth="1"/>
+    <col min="18" max="18" width="22" customWidth="1"/>
     <col min="19" max="19" width="17.5703125" customWidth="1"/>
     <col min="20" max="20" width="56.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.42578125" customWidth="1"/>
@@ -2772,1414 +2755,1414 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="4">
+        <v>914049118</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="4">
+        <v>28017</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="P2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>915220070</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="4">
+        <v>28004</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="4">
+        <v>915930540</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="4">
+        <v>28015</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="4">
+        <v>914379815</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="4">
+        <v>28030</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="P5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="4">
+        <v>644882198</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="4">
+        <v>28038</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="V6" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="4">
+        <v>913555550</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" s="4">
+        <v>28028</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="V7" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="4">
+        <v>635736573</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="4">
+        <v>28029</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="P8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="V8" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="4">
+        <v>914672726</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="4">
+        <v>28045</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11">
+      <c r="M9" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="V9" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4">
+        <v>917772822</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" s="4">
+        <v>28018</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="6">
-        <v>914049118</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="L10" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="V10" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="4">
+        <v>28014</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="L11" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="G2" s="6">
-        <v>28017</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="V11" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4">
+        <v>913721506</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="4">
+        <v>28029</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="6" t="b">
+      <c r="J12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L12" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="P12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="V12" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="4">
+        <v>28020</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="V13" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="4">
+        <v>914299756</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" s="4">
+        <v>28014</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="V14" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="4">
+        <v>913806604</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G15" s="4">
+        <v>28038</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="V15" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="4">
+        <v>918286978</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="4">
+        <v>28005</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="V16" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="4">
+        <v>915211174</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17" s="4">
+        <v>28012</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K17" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="U17" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="V17" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="4">
+        <v>28029</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="U18" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="V18" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="4">
+        <v>917779661</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="4">
+        <v>28038</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K19" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="P2" s="7" t="b">
+      <c r="M19" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="P19" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q2" s="7" t="b">
+      <c r="Q19" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R2" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="V2" s="13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6">
-        <v>915220070</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="6">
-        <v>28004</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="R19" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="U19" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="V19" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20" s="4">
+        <v>28012</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I20" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" s="6" t="b">
+      <c r="J20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K20" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L20" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="M3" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="O3" s="7" t="s">
+      <c r="M20" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="U20" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="V20" s="9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="4">
+        <v>915592906</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" s="4">
+        <v>28012</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K21" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="V21" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="4">
+        <v>912244837</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" s="4">
+        <v>28039</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K22" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="O22" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="V3" s="13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="6">
-        <v>915930540</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="G4" s="6">
-        <v>28015</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="P22" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="V22" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="10">
+        <v>22</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="11">
+        <v>911684483</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="11">
+        <v>28029</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I23" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J23" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="K4" s="6" t="b">
+      <c r="K23" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="V4" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="6">
-        <v>914379815</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="6">
-        <v>28030</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="O5" s="7" t="s">
+      <c r="L23" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="O23" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="P5" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="V5" s="13" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="6">
-        <v>644882198</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G6" s="6">
-        <v>28038</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="K6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="R6" s="7"/>
-      <c r="S6" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="U6" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="V6" s="13" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="6">
-        <v>913555550</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="G7" s="6">
-        <v>28028</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K7" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="V7" s="13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="6">
-        <v>635736573</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G8" s="6">
-        <v>28029</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="K8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P8" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="U8" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="V8" s="13" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="6">
-        <v>914672726</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="G9" s="6">
-        <v>28045</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K9" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="U9" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="V9" s="13" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="6">
-        <v>917772822</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G10" s="6">
-        <v>28018</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K10" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="U10" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="V10" s="13" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G11" s="6">
-        <v>28014</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="K11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="R11" s="7"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="U11" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="V11" s="13" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="6">
-        <v>913721506</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="G12" s="6">
-        <v>28029</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K12" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P12" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="U12" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="V12" s="13" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="G13" s="6">
-        <v>28020</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="K13" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="U13" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="V13" s="13" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="6">
-        <v>914299756</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="G14" s="6">
-        <v>28014</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K14" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="O14" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="R14" s="7"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="U14" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="V14" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="6">
-        <v>913806604</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="G15" s="6">
-        <v>28038</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K15" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="O15" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="U15" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="V15" s="13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="6">
-        <v>918286978</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="G16" s="6">
-        <v>28005</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="K16" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="U16" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="V16" s="13" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11">
-        <v>16</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="6">
-        <v>915211174</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G17" s="6">
-        <v>28012</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K17" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="M17" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="O17" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="T17" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="U17" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="V17" s="13" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11">
-        <v>17</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="G18" s="6">
-        <v>28029</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K18" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="M18" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="N18" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="O18" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="U18" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="V18" s="13" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11">
-        <v>18</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" s="6">
-        <v>917779661</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" s="6">
-        <v>28038</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="K19" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="O19" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P19" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="S19" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="T19" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="U19" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="V19" s="13" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="G20" s="6">
-        <v>28012</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K20" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="M20" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="N20" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="O20" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="U20" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="V20" s="13" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="6">
-        <v>915592906</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="G21" s="6">
-        <v>28012</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="K21" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="M21" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="O21" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="U21" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="V21" s="13" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11">
-        <v>21</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="6">
-        <v>912244837</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="G22" s="6">
-        <v>28039</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="K22" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="M22" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="N22" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="O22" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P22" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="U22" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="V22" s="13" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="14">
-        <v>22</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="15">
-        <v>911684483</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" s="15">
-        <v>28029</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="K23" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L23" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="M23" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="N23" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="O23" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15" t="s">
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="U23" s="15" t="s">
+      <c r="U23" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="V23" s="17" t="s">
+      <c r="V23" s="12" t="s">
         <v>200</v>
       </c>
     </row>
@@ -4194,10 +4177,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4292A902-63B0-4C12-AB71-49E517B57155}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4210,199 +4193,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="str">
-        <f t="shared" ref="A2:A11" si="0">IF(COUNTA($B2:$E2)&gt;0,CONCATENATE("cat",ROW($A2)-1),"Fill in the labels!")</f>
+      <c r="A2" s="2" t="str">
+        <f t="shared" ref="A2:A7" si="0">IF(COUNTA($B2:$E2)&gt;0,CONCATENATE("cat",ROW($A2)-1),"Fill in the labels!")</f>
         <v>cat1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="str">
+      <c r="A3" s="2" t="str">
         <f t="shared" si="0"/>
         <v>cat2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="str">
+      <c r="A4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>cat3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="str">
+      <c r="A5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>cat4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="str">
+      <c r="A6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>cat5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="str">
+      <c r="A7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>cat6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>cat7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>cat8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>cat9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>cat10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>218</v>
       </c>
     </row>
@@ -4434,552 +4345,552 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="5" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="str">
+      <c r="A2" s="2" t="str">
         <f>IF(COUNTA($B2:$F2)&gt;0,CONCATENATE(SUBSTITUTE($B2,"cat","svc"),ROW($A2)-1),"Fill in the labels!")</f>
         <v>svc11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="str">
+      <c r="A3" s="2" t="str">
         <f t="shared" ref="A3:A26" si="0">IF(COUNTA($B3:$F3)&gt;0,CONCATENATE(SUBSTITUTE($B3,"cat","svc"),ROW($A3)-1),"Fill in the labels!")</f>
         <v>svc12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="str">
+      <c r="A4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc13</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="str">
+      <c r="A5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc14</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="str">
+      <c r="A6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc15</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="str">
+      <c r="A7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="str">
+      <c r="A8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc27</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="str">
+      <c r="A9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc28</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="str">
+      <c r="A10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc29</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="str">
+      <c r="A11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc210</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="str">
+      <c r="A12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc211</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="str">
+      <c r="A13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc212</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="str">
+      <c r="A14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc213</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="str">
+      <c r="A15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc214</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="str">
+      <c r="A16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc215</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="str">
+      <c r="A17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc316</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="str">
+      <c r="A18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc317</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="str">
+      <c r="A19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc318</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="str">
+      <c r="A20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc319</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="str">
+      <c r="A21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc320</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="str">
+      <c r="A22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc321</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="str">
+      <c r="A23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc422</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="str">
+      <c r="A24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc423</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="str">
+      <c r="A25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc424</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="str">
+      <c r="A26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>svc425</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
+      <c r="A27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5019,70 +4930,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>218</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed link between map and table results. Added basic support for multi-languages
</commit_message>
<xml_diff>
--- a/excel-to-json/data.xlsx
+++ b/excel-to-json/data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Carlos\MadridForAll\madrid-for-all\excel-to-json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCC5662-66FF-42E6-B6D4-E5ACCE2597D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28908111-77C2-491C-A8A1-AAFDC39EFAA8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
     <sheet name="Services" sheetId="3" r:id="rId3"/>
     <sheet name="WaysOfContact" sheetId="4" r:id="rId4"/>
+    <sheet name="TargettedOrigins" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Categories!$A$1:$E$7</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="309">
   <si>
     <t>aem@alternativaenmarcha.org</t>
   </si>
@@ -361,15 +362,9 @@
     <t>district</t>
   </si>
   <si>
-    <t>timeTable</t>
-  </si>
-  <si>
     <t>priorAppointment</t>
   </si>
   <si>
-    <t>additionalInfo</t>
-  </si>
-  <si>
     <t>fullAddress</t>
   </si>
   <si>
@@ -923,6 +918,51 @@
   </si>
   <si>
     <t>PE;EQ</t>
+  </si>
+  <si>
+    <t>timeTable.ES</t>
+  </si>
+  <si>
+    <t>timeTable.EN</t>
+  </si>
+  <si>
+    <t>timeTable.FR</t>
+  </si>
+  <si>
+    <t>timeTable.AR</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>additionalInfo.ES</t>
+  </si>
+  <si>
+    <t>additionalInfo.EN</t>
+  </si>
+  <si>
+    <t>additionalInfo.FR</t>
+  </si>
+  <si>
+    <t>additionalInfo.AR</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Pérou</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
   </si>
 </sst>
 </file>
@@ -968,15 +1008,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1069,11 +1115,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1087,11 +1144,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="55">
     <dxf>
       <font>
         <b val="0"/>
@@ -1779,6 +1839,108 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1920,6 +2082,108 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2336,8 +2600,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{496FABF9-B904-41A0-9A3A-69F72B1F559C}">
-      <tableStyleElement type="wholeTable" dxfId="48"/>
-      <tableStyleElement type="headerRow" dxfId="47"/>
+      <tableStyleElement type="wholeTable" dxfId="54"/>
+      <tableStyleElement type="headerRow" dxfId="53"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2352,28 +2616,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA63940B-6736-4FFE-A90E-7DD2482B386E}" name="Table356" displayName="Table356" ref="A1:V23" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" tableBorderDxfId="44">
-  <autoFilter ref="A1:V23" xr:uid="{A1ABD4CF-8797-418F-84EC-F4D4132E0C98}"/>
-  <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{3CB7DF17-C103-48B7-B2BB-C03CA4ACA952}" name="ID" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{CB14816A-3E7B-4E30-B665-DD7CC64FC8FD}" name="orgName" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{9EE72959-C45C-47E7-921A-B7773AE82B21}" name="orgPhone" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{B008E3AC-8AAE-4D58-83F7-27986BD47CA6}" name="orgEmail" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{1CA78420-0C1C-4253-AE52-9F41B8939CA9}" name="orgWeb" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{68707F56-DA94-4407-B912-2963135E1136}" name="address" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{1AA6B013-D85D-417E-9A62-EF126E1AE66C}" name="postalCode" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{7D5976D5-FD34-4EBF-BA5B-F1BD6A5FCA4A}" name="district" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{4936B07E-6796-4057-A7AF-F9A5D9C459DC}" name="locality" dataDxfId="35"/>
-    <tableColumn id="10" xr3:uid="{E2316772-3F2F-415B-ACD3-89401FE74A44}" name="timeTable" dataDxfId="34"/>
-    <tableColumn id="11" xr3:uid="{756F15D8-2937-48DB-928D-C481CF43D8C2}" name="priorAppointment" dataDxfId="33"/>
-    <tableColumn id="12" xr3:uid="{0787C7F9-7719-46E1-A52B-0B7D48AD2DC0}" name="waysOfContact[]" dataDxfId="32"/>
-    <tableColumn id="13" xr3:uid="{2F4C62C8-2BEC-48D9-AD1F-00381CE97362}" name="categories[]" dataDxfId="31"/>
-    <tableColumn id="14" xr3:uid="{CD5E1452-5F2C-4B7B-8A48-81627D7F629E}" name="services[]" dataDxfId="30"/>
-    <tableColumn id="15" xr3:uid="{8AFE3F12-BA0B-42D4-A913-A52314BBCAF4}" name="languages[]" dataDxfId="29"/>
-    <tableColumn id="16" xr3:uid="{89630743-4A48-4707-AC78-3F737BCC5DFC}" name="targettedChild" dataDxfId="28"/>
-    <tableColumn id="17" xr3:uid="{47BB8DC5-0D94-41D6-ABA9-98DD02A8A0B1}" name="targettedWomen" dataDxfId="27"/>
-    <tableColumn id="18" xr3:uid="{C1678D26-A0C0-446D-8239-C35E55E07D73}" name="targettedOrigins[]" dataDxfId="26"/>
-    <tableColumn id="20" xr3:uid="{30A58EE2-5025-4DEE-B2E8-828F12E9E6A6}" name="additionalInfo" dataDxfId="25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA63940B-6736-4FFE-A90E-7DD2482B386E}" name="Table356" displayName="Table356" ref="A1:AB23" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51" tableBorderDxfId="50">
+  <autoFilter ref="A1:AB23" xr:uid="{A1ABD4CF-8797-418F-84EC-F4D4132E0C98}"/>
+  <tableColumns count="28">
+    <tableColumn id="1" xr3:uid="{3CB7DF17-C103-48B7-B2BB-C03CA4ACA952}" name="ID" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{CB14816A-3E7B-4E30-B665-DD7CC64FC8FD}" name="orgName" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{9EE72959-C45C-47E7-921A-B7773AE82B21}" name="orgPhone" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{B008E3AC-8AAE-4D58-83F7-27986BD47CA6}" name="orgEmail" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{1CA78420-0C1C-4253-AE52-9F41B8939CA9}" name="orgWeb" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{68707F56-DA94-4407-B912-2963135E1136}" name="address" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{1AA6B013-D85D-417E-9A62-EF126E1AE66C}" name="postalCode" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{7D5976D5-FD34-4EBF-BA5B-F1BD6A5FCA4A}" name="district" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{4936B07E-6796-4057-A7AF-F9A5D9C459DC}" name="locality" dataDxfId="41"/>
+    <tableColumn id="19" xr3:uid="{8513CE92-84E3-4FA2-BA35-0CD887298CEC}" name="timeTable.ES" dataDxfId="40"/>
+    <tableColumn id="22" xr3:uid="{B2B62B92-F903-4240-887D-C702DA204A0A}" name="timeTable.EN" dataDxfId="39"/>
+    <tableColumn id="21" xr3:uid="{5B214EDE-F533-4B25-8918-D5DECF46BBEB}" name="timeTable.FR" dataDxfId="38"/>
+    <tableColumn id="10" xr3:uid="{E2316772-3F2F-415B-ACD3-89401FE74A44}" name="timeTable.AR" dataDxfId="37"/>
+    <tableColumn id="11" xr3:uid="{756F15D8-2937-48DB-928D-C481CF43D8C2}" name="priorAppointment" dataDxfId="36"/>
+    <tableColumn id="12" xr3:uid="{0787C7F9-7719-46E1-A52B-0B7D48AD2DC0}" name="waysOfContact[]" dataDxfId="35"/>
+    <tableColumn id="13" xr3:uid="{2F4C62C8-2BEC-48D9-AD1F-00381CE97362}" name="categories[]" dataDxfId="34"/>
+    <tableColumn id="14" xr3:uid="{CD5E1452-5F2C-4B7B-8A48-81627D7F629E}" name="services[]" dataDxfId="33"/>
+    <tableColumn id="15" xr3:uid="{8AFE3F12-BA0B-42D4-A913-A52314BBCAF4}" name="languages[]" dataDxfId="32"/>
+    <tableColumn id="16" xr3:uid="{89630743-4A48-4707-AC78-3F737BCC5DFC}" name="targettedChild" dataDxfId="31"/>
+    <tableColumn id="17" xr3:uid="{47BB8DC5-0D94-41D6-ABA9-98DD02A8A0B1}" name="targettedWomen" dataDxfId="30"/>
+    <tableColumn id="18" xr3:uid="{C1678D26-A0C0-446D-8239-C35E55E07D73}" name="targettedOrigins[]" dataDxfId="29"/>
+    <tableColumn id="28" xr3:uid="{BC301DA3-1153-43AD-B2D8-5E0D3E1222E2}" name="additionalInfo.ES" dataDxfId="28"/>
+    <tableColumn id="27" xr3:uid="{C0629BDB-2103-45CC-99AD-87B828088F88}" name="additionalInfo.EN" dataDxfId="27"/>
+    <tableColumn id="23" xr3:uid="{FEE1C06C-6408-4478-9A95-BB6BF94E8F7B}" name="additionalInfo.FR" dataDxfId="26"/>
+    <tableColumn id="20" xr3:uid="{30A58EE2-5025-4DEE-B2E8-828F12E9E6A6}" name="additionalInfo.AR" dataDxfId="25"/>
     <tableColumn id="24" xr3:uid="{1D038E44-40C3-425C-A8C1-32D782986A58}" name="fullAddress" dataDxfId="24"/>
     <tableColumn id="25" xr3:uid="{C9080C18-D97E-4347-A518-16763BF326D2}" name="geocode.lat" dataDxfId="23"/>
     <tableColumn id="26" xr3:uid="{B2CBB689-92E1-4156-9126-3417F38FA8D2}" name="geocode.lng" dataDxfId="22"/>
@@ -2729,32 +2999,34 @@
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H5" sqref="H5"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="28.85546875" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.85546875" customWidth="1"/>
-    <col min="18" max="18" width="22" customWidth="1"/>
-    <col min="19" max="19" width="17.5703125" customWidth="1"/>
-    <col min="20" max="20" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="19" max="19" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.85546875" customWidth="1"/>
+    <col min="21" max="24" width="22" customWidth="1"/>
+    <col min="25" max="25" width="23" customWidth="1"/>
+    <col min="26" max="26" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.42578125" customWidth="1"/>
+    <col min="28" max="28" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>92</v>
       </c>
@@ -2780,49 +3052,67 @@
         <v>107</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="O1" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="Z1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -2839,7 +3129,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G2" s="4">
         <v>28017</v>
@@ -2848,47 +3138,65 @@
         <v>45</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="4" t="b">
+      <c r="K2" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N2" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>259</v>
-      </c>
       <c r="O2" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="P2" s="4" t="b">
+        <v>278</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="S2" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q2" s="4" t="b">
+      <c r="T2" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R2" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="U2" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -2914,45 +3222,63 @@
         <v>48</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="4" t="b">
+      <c r="K3" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N3" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>260</v>
-      </c>
       <c r="O3" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
+        <v>275</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>258</v>
+      </c>
       <c r="R3" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="S3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="V3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="T3" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="V3" s="9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W3" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -2969,7 +3295,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G4" s="4">
         <v>28015</v>
@@ -2978,43 +3304,61 @@
         <v>52</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="K4" s="4" t="b">
+      <c r="K4" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N4" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>261</v>
-      </c>
       <c r="O4" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="T4" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="V4" s="9" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W4" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB4" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -3038,43 +3382,61 @@
         <v>57</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="K5" s="4" t="b">
+      <c r="K5" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N5" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>262</v>
-      </c>
       <c r="O5" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P5" s="4" t="b">
+        <v>279</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="S5" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="U5" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="V5" s="9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB5" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -3100,43 +3462,61 @@
         <v>60</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K6" s="4" t="b">
+      <c r="K6" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N6" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L6" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="N6" s="4"/>
       <c r="O6" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4" t="b">
+        <v>279</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4" t="s">
+      <c r="U6" s="4"/>
+      <c r="V6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="T6" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="U6" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="V6" s="9" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W6" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB6" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -3153,48 +3533,66 @@
         <v>11</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G7" s="4">
         <v>28028</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="K7" s="4" t="b">
+      <c r="K7" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N7" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L7" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="N7" s="4"/>
       <c r="O7" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="P7" s="4"/>
+        <v>279</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>252</v>
+      </c>
       <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
+      <c r="R7" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="S7" s="4"/>
-      <c r="T7" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="U7" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="V7" s="9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB7" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -3209,7 +3607,7 @@
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G8" s="4">
         <v>28029</v>
@@ -3218,43 +3616,61 @@
         <v>65</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="K8" s="4" t="b">
+      <c r="K8" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N8" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L8" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>264</v>
-      </c>
       <c r="O8" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P8" s="4" t="b">
+        <v>280</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="S8" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="U8" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="V8" s="9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X8" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y8" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA8" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB8" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -3271,7 +3687,7 @@
         <v>90</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G9" s="4">
         <v>28045</v>
@@ -3280,43 +3696,61 @@
         <v>68</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="4" t="b">
+      <c r="K9" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N9" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L9" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>265</v>
-      </c>
       <c r="O9" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
+        <v>281</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>263</v>
+      </c>
       <c r="R9" s="4" t="s">
-        <v>287</v>
+        <v>125</v>
       </c>
       <c r="S9" s="4"/>
-      <c r="T9" s="4" t="s">
-        <v>141</v>
-      </c>
+      <c r="T9" s="4"/>
       <c r="U9" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="V9" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X9" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y9" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA9" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB9" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -3333,7 +3767,7 @@
         <v>16</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G10" s="4">
         <v>28018</v>
@@ -3342,41 +3776,59 @@
         <v>60</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K10" s="4" t="b">
+      <c r="K10" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N10" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L10" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>266</v>
-      </c>
       <c r="O10" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
+        <v>280</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="S10" s="4"/>
-      <c r="T10" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="U10" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="V10" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA10" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB10" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -3400,43 +3852,61 @@
         <v>48</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K11" s="4" t="b">
+      <c r="K11" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N11" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L11" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>267</v>
-      </c>
       <c r="O11" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4" t="b">
+        <v>279</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="V11" s="9" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y11" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z11" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA11" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB11" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -3462,45 +3932,63 @@
         <v>65</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="K12" s="4" t="b">
+      <c r="K12" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N12" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L12" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>267</v>
-      </c>
       <c r="O12" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P12" s="4" t="b">
+        <v>275</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="S12" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4" t="s">
-        <v>144</v>
-      </c>
+      <c r="T12" s="4"/>
       <c r="U12" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="V12" s="9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>283</v>
+      </c>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X12" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y12" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA12" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB12" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -3524,41 +4012,59 @@
         <v>72</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="4" t="b">
+      <c r="K13" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N13" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L13" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>268</v>
-      </c>
       <c r="O13" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
+        <v>279</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="S13" s="4"/>
-      <c r="T13" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="U13" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="V13" s="9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X13" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y13" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA13" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB13" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -3575,7 +4081,7 @@
         <v>25</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G14" s="4">
         <v>28014</v>
@@ -3584,43 +4090,61 @@
         <v>48</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="K14" s="4" t="b">
+      <c r="K14" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L14" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>269</v>
-      </c>
       <c r="O14" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4" t="b">
+        <v>279</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="U14" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="V14" s="9" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA14" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB14" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -3637,7 +4161,7 @@
         <v>27</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G15" s="4">
         <v>28038</v>
@@ -3646,43 +4170,61 @@
         <v>60</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K15" s="4" t="b">
+      <c r="K15" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N15" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L15" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>270</v>
-      </c>
       <c r="O15" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
+        <v>279</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>268</v>
+      </c>
       <c r="R15" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="S15" s="4"/>
-      <c r="T15" s="4" t="s">
-        <v>147</v>
-      </c>
+      <c r="T15" s="4"/>
       <c r="U15" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="V15" s="9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y15" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA15" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AB15" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -3699,7 +4241,7 @@
         <v>29</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G16" s="4">
         <v>28005</v>
@@ -3708,39 +4250,57 @@
         <v>68</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="K16" s="4" t="b">
+      <c r="K16" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N16" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L16" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="N16" s="4"/>
       <c r="O16" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P16" s="4"/>
+        <v>280</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>207</v>
+      </c>
       <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
+      <c r="R16" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="S16" s="4"/>
-      <c r="T16" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="U16" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="V16" s="9" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y16" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA16" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB16" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -3757,7 +4317,7 @@
         <v>31</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G17" s="4">
         <v>28012</v>
@@ -3766,43 +4326,61 @@
         <v>48</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="K17" s="4" t="b">
+      <c r="K17" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N17" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L17" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>263</v>
-      </c>
       <c r="O17" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="T17" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="U17" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="V17" s="9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W17" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X17" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y17" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z17" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA17" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB17" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -3826,41 +4404,59 @@
         <v>72</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="K18" s="4" t="b">
+      <c r="K18" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N18" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L18" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>271</v>
-      </c>
       <c r="O18" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
+        <v>276</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="S18" s="4"/>
-      <c r="T18" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="U18" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="V18" s="9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X18" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y18" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z18" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA18" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB18" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -3884,49 +4480,67 @@
         <v>60</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="K19" s="4" t="b">
+      <c r="K19" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N19" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="O19" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="S19" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T19" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="U19" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="M19" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="O19" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P19" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="R19" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="S19" s="4" t="s">
+      <c r="V19" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="T19" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="U19" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="V19" s="9" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W19" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X19" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y19" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z19" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA19" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="AB19" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -3941,7 +4555,7 @@
         <v>36</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G20" s="4">
         <v>28012</v>
@@ -3950,41 +4564,59 @@
         <v>48</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="K20" s="4" t="b">
+      <c r="K20" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N20" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L20" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>273</v>
-      </c>
       <c r="O20" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
+        <v>279</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="S20" s="4"/>
-      <c r="T20" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="U20" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="V20" s="9" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X20" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y20" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA20" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="AB20" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -4001,7 +4633,7 @@
         <v>38</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G21" s="4">
         <v>28012</v>
@@ -4010,41 +4642,59 @@
         <v>48</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="K21" s="4" t="b">
+      <c r="K21" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N21" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L21" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>274</v>
-      </c>
       <c r="O21" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
+        <v>275</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="S21" s="4"/>
-      <c r="T21" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="U21" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="V21" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X21" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y21" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z21" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA21" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AB21" s="9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -4070,43 +4720,61 @@
         <v>88</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="K22" s="4" t="b">
+      <c r="K22" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N22" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L22" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>275</v>
-      </c>
       <c r="O22" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P22" s="4" t="b">
+        <v>286</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="S22" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="U22" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="V22" s="9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X22" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y22" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z22" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA22" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB22" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -4132,38 +4800,56 @@
         <v>72</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J23" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="K23" s="11" t="b">
+      <c r="K23" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N23" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="L23" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>276</v>
-      </c>
       <c r="O23" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
+        <v>275</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="R23" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="S23" s="11"/>
-      <c r="T23" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="U23" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="V23" s="12" t="s">
-        <v>200</v>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="X23" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y23" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z23" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA23" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB23" s="12" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -4179,8 +4865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4292A902-63B0-4C12-AB71-49E517B57155}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4194,19 +4880,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -4215,16 +4901,16 @@
         <v>cat1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -4233,16 +4919,16 @@
         <v>cat2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -4251,16 +4937,16 @@
         <v>cat3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -4269,16 +4955,16 @@
         <v>cat4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -4287,16 +4973,16 @@
         <v>cat5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -4305,16 +4991,16 @@
         <v>cat6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -4328,11 +5014,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8087170B-0D62-4A26-AF96-7842979EAF6C}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4346,22 +5030,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -4370,19 +5054,19 @@
         <v>svc11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -4391,19 +5075,19 @@
         <v>svc12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -4412,19 +5096,19 @@
         <v>svc13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -4433,19 +5117,19 @@
         <v>svc14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -4454,19 +5138,19 @@
         <v>svc15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -4475,19 +5159,19 @@
         <v>svc16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -4496,19 +5180,19 @@
         <v>svc27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -4517,19 +5201,19 @@
         <v>svc28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -4538,19 +5222,19 @@
         <v>svc29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -4559,19 +5243,19 @@
         <v>svc210</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -4580,19 +5264,19 @@
         <v>svc211</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -4601,19 +5285,19 @@
         <v>svc212</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -4622,19 +5306,19 @@
         <v>svc213</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -4643,19 +5327,19 @@
         <v>svc214</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -4664,19 +5348,19 @@
         <v>svc215</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -4685,19 +5369,19 @@
         <v>svc316</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -4706,19 +5390,19 @@
         <v>svc317</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -4727,19 +5411,19 @@
         <v>svc318</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -4748,19 +5432,19 @@
         <v>svc319</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -4769,19 +5453,19 @@
         <v>svc320</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -4790,19 +5474,19 @@
         <v>svc321</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -4811,19 +5495,19 @@
         <v>svc422</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -4832,19 +5516,19 @@
         <v>svc423</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -4853,19 +5537,19 @@
         <v>svc424</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -4874,23 +5558,20 @@
         <v>svc425</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
+        <v>216</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4918,7 +5599,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4931,70 +5612,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -5004,4 +5685,70 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4532F6C8-4F1F-4B5E-A128-E84586164F62}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added all the missing translations. Fixed issue with orgWeb in popup
</commit_message>
<xml_diff>
--- a/excel-to-json/data.xlsx
+++ b/excel-to-json/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Carlos\MadridForAll\madrid-for-all\excel-to-json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE156C8C-BCC0-4DA3-8E5D-39D84D39BD66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394EEC25-CE89-4FD5-9AC7-B1FABCE35FCB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -3182,9 +3182,6 @@
     <t>Voluntary termination of pregnancy</t>
   </si>
   <si>
-    <t>orgweb</t>
-  </si>
-  <si>
     <t>www.asociacionrealidades.org</t>
   </si>
   <si>
@@ -3411,6 +3408,9 @@
   </si>
   <si>
     <t>Translation / Mediation</t>
+  </si>
+  <si>
+    <t>orgWeb</t>
   </si>
 </sst>
 </file>
@@ -4001,9 +4001,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AA65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4048,7 +4048,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1004</v>
+        <v>1080</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -4177,7 +4177,7 @@
       <c r="W2" s="19"/>
       <c r="X2" s="16"/>
       <c r="Y2" s="19" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="Z2" s="22" t="s">
         <v>882</v>
@@ -4252,7 +4252,7 @@
         <v>119</v>
       </c>
       <c r="Y3" s="19" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="Z3" s="22" t="s">
         <v>980</v>
@@ -4325,7 +4325,7 @@
         <v>133</v>
       </c>
       <c r="Y4" s="19" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="Z4" s="22" t="s">
         <v>884</v>
@@ -4400,13 +4400,13 @@
         <v>140</v>
       </c>
       <c r="Y5" s="19" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="Z5" s="22" t="s">
         <v>884</v>
       </c>
       <c r="AA5" s="23" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4469,7 +4469,7 @@
       <c r="W6" s="19"/>
       <c r="X6" s="16"/>
       <c r="Y6" s="19" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="Z6" s="22" t="s">
         <v>886</v>
@@ -4544,7 +4544,7 @@
         <v>863</v>
       </c>
       <c r="Y7" s="19" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="Z7" s="22" t="s">
         <v>888</v>
@@ -4623,7 +4623,7 @@
         <v>210</v>
       </c>
       <c r="Y8" s="19" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="Z8" s="22" t="s">
         <v>982</v>
@@ -4690,7 +4690,7 @@
       <c r="W9" s="19"/>
       <c r="X9" s="16"/>
       <c r="Y9" s="19" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="Z9" s="22" t="s">
         <v>886</v>
@@ -4713,7 +4713,7 @@
         <v>221</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>222</v>
@@ -4765,7 +4765,7 @@
         <v>232</v>
       </c>
       <c r="Y10" s="19" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="Z10" s="22" t="s">
         <v>985</v>
@@ -4834,7 +4834,7 @@
       <c r="W11" s="19"/>
       <c r="X11" s="16"/>
       <c r="Y11" s="19" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="Z11" s="22" t="s">
         <v>890</v>
@@ -4905,7 +4905,7 @@
         <v>248</v>
       </c>
       <c r="Y12" s="19" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="Z12" s="22" t="s">
         <v>892</v>
@@ -4982,7 +4982,7 @@
         <v>257</v>
       </c>
       <c r="Y13" s="19" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="Z13" s="22" t="s">
         <v>894</v>
@@ -5047,7 +5047,7 @@
       <c r="W14" s="19"/>
       <c r="X14" s="16"/>
       <c r="Y14" s="19" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="Z14" s="22" t="s">
         <v>896</v>
@@ -5116,7 +5116,7 @@
       <c r="W15" s="19"/>
       <c r="X15" s="16"/>
       <c r="Y15" s="19" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="Z15" s="22" t="s">
         <v>898</v>
@@ -5264,7 +5264,7 @@
         <v>315</v>
       </c>
       <c r="Y17" s="19" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="Z17" s="22" t="s">
         <v>971</v>
@@ -5331,7 +5331,7 @@
       <c r="W18" s="19"/>
       <c r="X18" s="16"/>
       <c r="Y18" s="19" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="Z18" s="22" t="s">
         <v>902</v>
@@ -5404,7 +5404,7 @@
         <v>359</v>
       </c>
       <c r="Y19" s="19" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="Z19" s="22" t="s">
         <v>988</v>
@@ -5479,7 +5479,7 @@
         <v>375</v>
       </c>
       <c r="Y20" s="19" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="Z20" s="22" t="s">
         <v>904</v>
@@ -5554,7 +5554,7 @@
         <v>359</v>
       </c>
       <c r="Y21" s="25" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="Z21" s="22" t="s">
         <v>906</v>
@@ -5629,7 +5629,7 @@
         <v>468</v>
       </c>
       <c r="Y22" s="19" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="Z22" s="22" t="s">
         <v>990</v>
@@ -5698,7 +5698,7 @@
       <c r="W23" s="19"/>
       <c r="X23" s="16"/>
       <c r="Y23" s="19" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="Z23" s="22" t="s">
         <v>908</v>
@@ -5775,7 +5775,7 @@
         <v>487</v>
       </c>
       <c r="Y24" s="19" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="Z24" s="22" t="s">
         <v>910</v>
@@ -5852,7 +5852,7 @@
         <v>487</v>
       </c>
       <c r="Y25" s="19" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="Z25" s="22" t="s">
         <v>912</v>
@@ -5931,7 +5931,7 @@
         <v>501</v>
       </c>
       <c r="Y26" s="19" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="Z26" s="22" t="s">
         <v>914</v>
@@ -6012,7 +6012,7 @@
         <v>512</v>
       </c>
       <c r="Y27" s="19" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="Z27" s="22" t="s">
         <v>916</v>
@@ -6089,7 +6089,7 @@
         <v>523</v>
       </c>
       <c r="Y28" s="19" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="Z28" s="22" t="s">
         <v>917</v>
@@ -6166,7 +6166,7 @@
         <v>533</v>
       </c>
       <c r="Y29" s="19" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="Z29" s="22" t="s">
         <v>919</v>
@@ -6397,7 +6397,7 @@
         <v>557</v>
       </c>
       <c r="Y32" s="19" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="Z32" s="22" t="s">
         <v>925</v>
@@ -6551,7 +6551,7 @@
         <v>574</v>
       </c>
       <c r="Y34" s="19" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="Z34" s="22" t="s">
         <v>994</v>
@@ -6626,7 +6626,7 @@
         <v>581</v>
       </c>
       <c r="Y35" s="19" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="Z35" s="22" t="s">
         <v>927</v>
@@ -6701,7 +6701,7 @@
         <v>588</v>
       </c>
       <c r="Y36" s="19" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="Z36" s="22" t="s">
         <v>929</v>
@@ -6778,7 +6778,7 @@
         <v>599</v>
       </c>
       <c r="Y37" s="19" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="Z37" s="22" t="s">
         <v>931</v>
@@ -6853,7 +6853,7 @@
         <v>611</v>
       </c>
       <c r="Y38" s="19" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="Z38" s="22" t="s">
         <v>933</v>
@@ -6926,7 +6926,7 @@
         <v>620</v>
       </c>
       <c r="Y39" s="19" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="Z39" s="22" t="s">
         <v>935</v>
@@ -7003,7 +7003,7 @@
         <v>627</v>
       </c>
       <c r="Y40" s="19" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="Z40" s="22" t="s">
         <v>937</v>
@@ -7076,7 +7076,7 @@
         <v>634</v>
       </c>
       <c r="Y41" s="19" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="Z41" s="22" t="s">
         <v>939</v>
@@ -7153,7 +7153,7 @@
         <v>873</v>
       </c>
       <c r="Y42" s="19" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="Z42" s="22" t="s">
         <v>941</v>
@@ -7222,7 +7222,7 @@
       <c r="W43" s="19"/>
       <c r="X43" s="16"/>
       <c r="Y43" s="19" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="Z43" s="22" t="s">
         <v>996</v>
@@ -7295,7 +7295,7 @@
         <v>659</v>
       </c>
       <c r="Y44" s="19" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="Z44" s="22" t="s">
         <v>943</v>
@@ -7370,7 +7370,7 @@
         <v>670</v>
       </c>
       <c r="Y45" s="19" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="Z45" s="22" t="s">
         <v>945</v>
@@ -7439,7 +7439,7 @@
       <c r="W46" s="19"/>
       <c r="X46" s="16"/>
       <c r="Y46" s="19" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="Z46" s="22" t="s">
         <v>947</v>
@@ -7514,7 +7514,7 @@
         <v>683</v>
       </c>
       <c r="Y47" s="19" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="Z47" s="22" t="s">
         <v>949</v>
@@ -7589,7 +7589,7 @@
         <v>692</v>
       </c>
       <c r="Y48" s="19" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="Z48" s="22" t="s">
         <v>951</v>
@@ -7666,7 +7666,7 @@
         <v>700</v>
       </c>
       <c r="Y49" s="19" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="Z49" s="22" t="s">
         <v>953</v>
@@ -7741,7 +7741,7 @@
         <v>711</v>
       </c>
       <c r="Y50" s="19" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="Z50" s="22" t="s">
         <v>998</v>
@@ -7816,7 +7816,7 @@
         <v>720</v>
       </c>
       <c r="Y51" s="19" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="Z51" s="22" t="s">
         <v>955</v>
@@ -7895,7 +7895,7 @@
         <v>732</v>
       </c>
       <c r="Y52" s="19" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="Z52" s="22" t="s">
         <v>957</v>
@@ -7972,7 +7972,7 @@
         <v>745</v>
       </c>
       <c r="Y53" s="19" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="Z53" s="22" t="s">
         <v>959</v>
@@ -8043,7 +8043,7 @@
       <c r="W54" s="19"/>
       <c r="X54" s="16"/>
       <c r="Y54" s="19" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="Z54" s="22" t="s">
         <v>961</v>
@@ -8120,7 +8120,7 @@
         <v>765</v>
       </c>
       <c r="Y55" s="19" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="Z55" s="22" t="s">
         <v>963</v>
@@ -8197,7 +8197,7 @@
         <v>779</v>
       </c>
       <c r="Y56" s="19" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="Z56" s="22" t="s">
         <v>978</v>
@@ -8276,7 +8276,7 @@
         <v>787</v>
       </c>
       <c r="Y57" s="19" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="Z57" s="22" t="s">
         <v>1000</v>
@@ -8299,7 +8299,7 @@
         <v>789</v>
       </c>
       <c r="E58" s="20" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="F58" s="19" t="s">
         <v>782</v>
@@ -8355,7 +8355,7 @@
         <v>794</v>
       </c>
       <c r="Y58" s="19" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="Z58" s="22" t="s">
         <v>1000</v>
@@ -8430,7 +8430,7 @@
         <v>804</v>
       </c>
       <c r="Y59" s="19" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="Z59" s="22" t="s">
         <v>965</v>
@@ -8505,7 +8505,7 @@
         <v>813</v>
       </c>
       <c r="Y60" s="19" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="Z60" s="22" t="s">
         <v>967</v>
@@ -8582,7 +8582,7 @@
         <v>821</v>
       </c>
       <c r="Y61" s="19" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="Z61" s="22" t="s">
         <v>969</v>
@@ -8659,7 +8659,7 @@
         <v>829</v>
       </c>
       <c r="Y62" s="19" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="Z62" s="22" t="s">
         <v>976</v>
@@ -8732,7 +8732,7 @@
         <v>836</v>
       </c>
       <c r="Y63" s="19" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="Z63" s="22" t="s">
         <v>971</v>
@@ -8805,7 +8805,7 @@
         <v>848</v>
       </c>
       <c r="Y64" s="19" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="Z64" s="22" t="s">
         <v>973</v>
@@ -8878,7 +8878,7 @@
         <v>857</v>
       </c>
       <c r="Y65" s="19" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="Z65" s="22" t="s">
         <v>973</v>
@@ -8903,7 +8903,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -8935,7 +8935,7 @@
         <v>31</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8955,7 +8955,7 @@
         <v>157</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8975,7 +8975,7 @@
         <v>157</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8995,7 +8995,7 @@
         <v>157</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9015,7 +9015,7 @@
         <v>157</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9035,7 +9035,7 @@
         <v>157</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9043,10 +9043,10 @@
         <v>181</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>182</v>
@@ -9055,7 +9055,7 @@
         <v>157</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9063,10 +9063,10 @@
         <v>185</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>187</v>
@@ -9075,7 +9075,7 @@
         <v>157</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9086,7 +9086,7 @@
         <v>189</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>190</v>
@@ -9095,7 +9095,7 @@
         <v>157</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9115,7 +9115,7 @@
         <v>157</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -9135,7 +9135,7 @@
         <v>157</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrated vue framework in the page
</commit_message>
<xml_diff>
--- a/excel-to-json/data.xlsx
+++ b/excel-to-json/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Carlos\MadridForAll\madrid-for-all\excel-to-json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4E9940-112E-48E7-BE67-97AC21E09B19}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7F2C27-131B-4AEA-A66C-A8F0B854EF86}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3992,9 +3992,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>